<commit_message>
Working on creating a master table
</commit_message>
<xml_diff>
--- a/sorted_salaries.xlsx
+++ b/sorted_salaries.xlsx
@@ -1,28 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28810"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikowhy/Documents/Informatyka/Side Projects/Python/PlaceToLive/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -1241,8 +1228,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1305,11 +1292,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1356,12 +1338,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1388,15 +1370,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1423,7 +1404,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1599,16 +1579,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E243"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1625,7 +1603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>210</v>
       </c>
@@ -1642,7 +1620,7 @@
         <v>11238</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>229</v>
       </c>
@@ -1659,7 +1637,7 @@
         <v>9489</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>58</v>
       </c>
@@ -1676,7 +1654,7 @@
         <v>7640</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>107</v>
       </c>
@@ -1693,7 +1671,7 @@
         <v>7502</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>125</v>
       </c>
@@ -1710,7 +1688,7 @@
         <v>7313</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>196</v>
       </c>
@@ -1727,7 +1705,7 @@
         <v>7226</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>162</v>
       </c>
@@ -1744,7 +1722,7 @@
         <v>7137</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>97</v>
       </c>
@@ -1761,7 +1739,7 @@
         <v>6883</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>228</v>
       </c>
@@ -1778,7 +1756,7 @@
         <v>6621</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>155</v>
       </c>
@@ -1795,7 +1773,7 @@
         <v>6545</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>99</v>
       </c>
@@ -1812,7 +1790,7 @@
         <v>6526</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>74</v>
       </c>
@@ -1829,7 +1807,7 @@
         <v>6522</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>123</v>
       </c>
@@ -1846,7 +1824,7 @@
         <v>6328</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>73</v>
       </c>
@@ -1863,7 +1841,7 @@
         <v>6081</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>45</v>
       </c>
@@ -1880,7 +1858,7 @@
         <v>6051</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>13</v>
       </c>
@@ -1897,7 +1875,7 @@
         <v>6024</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>81</v>
       </c>
@@ -1914,7 +1892,7 @@
         <v>5983</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>152</v>
       </c>
@@ -1931,7 +1909,7 @@
         <v>5814</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>209</v>
       </c>
@@ -1948,7 +1926,7 @@
         <v>5620</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>87</v>
       </c>
@@ -1965,7 +1943,7 @@
         <v>5430</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>163</v>
       </c>
@@ -1982,7 +1960,7 @@
         <v>5428</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>38</v>
       </c>
@@ -1999,7 +1977,7 @@
         <v>5361</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>21</v>
       </c>
@@ -2016,7 +1994,7 @@
         <v>5359</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>191</v>
       </c>
@@ -2033,7 +2011,7 @@
         <v>5260</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>177</v>
       </c>
@@ -2050,7 +2028,7 @@
         <v>5232</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>176</v>
       </c>
@@ -2067,7 +2045,7 @@
         <v>5087</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>71</v>
       </c>
@@ -2084,7 +2062,7 @@
         <v>5030</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>144</v>
       </c>
@@ -2101,7 +2079,7 @@
         <v>4924</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>83</v>
       </c>
@@ -2118,7 +2096,7 @@
         <v>4916</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>142</v>
       </c>
@@ -2135,7 +2113,7 @@
         <v>4914</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>14</v>
       </c>
@@ -2152,7 +2130,7 @@
         <v>4912</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>90</v>
       </c>
@@ -2169,7 +2147,7 @@
         <v>4912</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>115</v>
       </c>
@@ -2186,7 +2164,7 @@
         <v>4909</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>85</v>
       </c>
@@ -2203,7 +2181,7 @@
         <v>4903</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>227</v>
       </c>
@@ -2220,7 +2198,7 @@
         <v>4870</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>46</v>
       </c>
@@ -2237,7 +2215,7 @@
         <v>4846</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>44</v>
       </c>
@@ -2254,7 +2232,7 @@
         <v>4843</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>108</v>
       </c>
@@ -2271,7 +2249,7 @@
         <v>4826</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>105</v>
       </c>
@@ -2288,7 +2266,7 @@
         <v>4730</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>104</v>
       </c>
@@ -2305,7 +2283,7 @@
         <v>4725</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>2</v>
       </c>
@@ -2322,7 +2300,7 @@
         <v>4715</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>189</v>
       </c>
@@ -2339,7 +2317,7 @@
         <v>4705</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>160</v>
       </c>
@@ -2356,7 +2334,7 @@
         <v>4650</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>17</v>
       </c>
@@ -2373,7 +2351,7 @@
         <v>4631</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>40</v>
       </c>
@@ -2390,7 +2368,7 @@
         <v>4597</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47">
         <v>202</v>
       </c>
@@ -2407,7 +2385,7 @@
         <v>4496</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48">
         <v>217</v>
       </c>
@@ -2424,7 +2402,7 @@
         <v>4487</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>56</v>
       </c>
@@ -2441,7 +2419,7 @@
         <v>4413</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50">
         <v>186</v>
       </c>
@@ -2458,7 +2436,7 @@
         <v>4399</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>114</v>
       </c>
@@ -2475,7 +2453,7 @@
         <v>4253</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52">
         <v>185</v>
       </c>
@@ -2492,7 +2470,7 @@
         <v>4248</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="A53">
         <v>172</v>
       </c>
@@ -2509,7 +2487,7 @@
         <v>4243</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5">
       <c r="A54">
         <v>197</v>
       </c>
@@ -2526,7 +2504,7 @@
         <v>4149</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5">
       <c r="A55">
         <v>224</v>
       </c>
@@ -2543,7 +2521,7 @@
         <v>4146</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5">
       <c r="A56">
         <v>112</v>
       </c>
@@ -2560,7 +2538,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5">
       <c r="A57">
         <v>51</v>
       </c>
@@ -2577,7 +2555,7 @@
         <v>4075</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5">
       <c r="A58">
         <v>75</v>
       </c>
@@ -2594,7 +2572,7 @@
         <v>4062</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5">
       <c r="A59">
         <v>203</v>
       </c>
@@ -2611,7 +2589,7 @@
         <v>4046</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5">
       <c r="A60">
         <v>135</v>
       </c>
@@ -2628,7 +2606,7 @@
         <v>3903</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61">
         <v>39</v>
       </c>
@@ -2645,7 +2623,7 @@
         <v>3804</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="A62">
         <v>181</v>
       </c>
@@ -2662,7 +2640,7 @@
         <v>3793</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5">
       <c r="A63">
         <v>215</v>
       </c>
@@ -2679,7 +2657,7 @@
         <v>3764</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5">
       <c r="A64">
         <v>16</v>
       </c>
@@ -2696,7 +2674,7 @@
         <v>3738</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5">
       <c r="A65">
         <v>198</v>
       </c>
@@ -2713,7 +2691,7 @@
         <v>3707</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5">
       <c r="A66">
         <v>159</v>
       </c>
@@ -2730,7 +2708,7 @@
         <v>3696</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5">
       <c r="A67">
         <v>84</v>
       </c>
@@ -2747,7 +2725,7 @@
         <v>3658</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5">
       <c r="A68">
         <v>77</v>
       </c>
@@ -2764,7 +2742,7 @@
         <v>3634</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5">
       <c r="A69">
         <v>174</v>
       </c>
@@ -2781,7 +2759,7 @@
         <v>3623</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5">
       <c r="A70">
         <v>141</v>
       </c>
@@ -2798,7 +2776,7 @@
         <v>3621</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5">
       <c r="A71">
         <v>234</v>
       </c>
@@ -2815,7 +2793,7 @@
         <v>3621</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5">
       <c r="A72">
         <v>212</v>
       </c>
@@ -2832,7 +2810,7 @@
         <v>3582</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5">
       <c r="A73">
         <v>133</v>
       </c>
@@ -2849,7 +2827,7 @@
         <v>3478</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5">
       <c r="A74">
         <v>6</v>
       </c>
@@ -2866,7 +2844,7 @@
         <v>3383</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5">
       <c r="A75">
         <v>207</v>
       </c>
@@ -2883,7 +2861,7 @@
         <v>3375</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5">
       <c r="A76">
         <v>138</v>
       </c>
@@ -2900,7 +2878,7 @@
         <v>3355</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5">
       <c r="A77">
         <v>52</v>
       </c>
@@ -2917,7 +2895,7 @@
         <v>3329</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5">
       <c r="A78">
         <v>30</v>
       </c>
@@ -2934,7 +2912,7 @@
         <v>3247</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5">
       <c r="A79">
         <v>167</v>
       </c>
@@ -2951,7 +2929,7 @@
         <v>3148</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5">
       <c r="A80">
         <v>109</v>
       </c>
@@ -2968,7 +2946,7 @@
         <v>3139</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5">
       <c r="A81">
         <v>72</v>
       </c>
@@ -2985,7 +2963,7 @@
         <v>3117</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5">
       <c r="A82">
         <v>122</v>
       </c>
@@ -3002,7 +2980,7 @@
         <v>3100</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5">
       <c r="A83">
         <v>230</v>
       </c>
@@ -3019,7 +2997,7 @@
         <v>3085</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5">
       <c r="A84">
         <v>150</v>
       </c>
@@ -3036,7 +3014,7 @@
         <v>3041</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5">
       <c r="A85">
         <v>153</v>
       </c>
@@ -3053,7 +3031,7 @@
         <v>2948</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5">
       <c r="A86">
         <v>57</v>
       </c>
@@ -3070,7 +3048,7 @@
         <v>2927</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5">
       <c r="A87">
         <v>134</v>
       </c>
@@ -3087,7 +3065,7 @@
         <v>2924</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5">
       <c r="A88">
         <v>192</v>
       </c>
@@ -3104,7 +3082,7 @@
         <v>2918</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5">
       <c r="A89">
         <v>146</v>
       </c>
@@ -3121,7 +3099,7 @@
         <v>2913</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5">
       <c r="A90">
         <v>95</v>
       </c>
@@ -3138,7 +3116,7 @@
         <v>2905</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5">
       <c r="A91">
         <v>179</v>
       </c>
@@ -3155,7 +3133,7 @@
         <v>2847</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5">
       <c r="A92">
         <v>119</v>
       </c>
@@ -3172,7 +3150,7 @@
         <v>2812</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5">
       <c r="A93">
         <v>12</v>
       </c>
@@ -3189,7 +3167,7 @@
         <v>2763</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5">
       <c r="A94">
         <v>32</v>
       </c>
@@ -3206,7 +3184,7 @@
         <v>2750</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5">
       <c r="A95">
         <v>139</v>
       </c>
@@ -3223,7 +3201,7 @@
         <v>2736</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5">
       <c r="A96">
         <v>80</v>
       </c>
@@ -3240,7 +3218,7 @@
         <v>2687</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5">
       <c r="A97">
         <v>173</v>
       </c>
@@ -3257,7 +3235,7 @@
         <v>2675</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5">
       <c r="A98">
         <v>43</v>
       </c>
@@ -3274,7 +3252,7 @@
         <v>2660</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5">
       <c r="A99">
         <v>103</v>
       </c>
@@ -3291,7 +3269,7 @@
         <v>2580</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5">
       <c r="A100">
         <v>222</v>
       </c>
@@ -3308,7 +3286,7 @@
         <v>2506</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5">
       <c r="A101">
         <v>118</v>
       </c>
@@ -3325,7 +3303,7 @@
         <v>2476</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5">
       <c r="A102">
         <v>199</v>
       </c>
@@ -3342,7 +3320,7 @@
         <v>2471</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5">
       <c r="A103">
         <v>98</v>
       </c>
@@ -3359,7 +3337,7 @@
         <v>2440</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5">
       <c r="A104">
         <v>201</v>
       </c>
@@ -3376,7 +3354,7 @@
         <v>2410</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5">
       <c r="A105">
         <v>54</v>
       </c>
@@ -3393,7 +3371,7 @@
         <v>2297</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5">
       <c r="A106">
         <v>70</v>
       </c>
@@ -3410,7 +3388,7 @@
         <v>2264</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5">
       <c r="A107">
         <v>193</v>
       </c>
@@ -3427,7 +3405,7 @@
         <v>2261</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5">
       <c r="A108">
         <v>20</v>
       </c>
@@ -3444,7 +3422,7 @@
         <v>2233</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5">
       <c r="A109">
         <v>11</v>
       </c>
@@ -3461,7 +3439,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5">
       <c r="A110">
         <v>130</v>
       </c>
@@ -3478,7 +3456,7 @@
         <v>2199</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5">
       <c r="A111">
         <v>220</v>
       </c>
@@ -3495,7 +3473,7 @@
         <v>2193</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5">
       <c r="A112">
         <v>22</v>
       </c>
@@ -3512,7 +3490,7 @@
         <v>2177</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5">
       <c r="A113">
         <v>175</v>
       </c>
@@ -3529,7 +3507,7 @@
         <v>2175</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5">
       <c r="A114">
         <v>4</v>
       </c>
@@ -3546,7 +3524,7 @@
         <v>2147</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5">
       <c r="A115">
         <v>124</v>
       </c>
@@ -3563,7 +3541,7 @@
         <v>2084</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5">
       <c r="A116">
         <v>88</v>
       </c>
@@ -3580,7 +3558,7 @@
         <v>2057</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5">
       <c r="A117">
         <v>15</v>
       </c>
@@ -3597,7 +3575,7 @@
         <v>2043</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5">
       <c r="A118">
         <v>48</v>
       </c>
@@ -3614,7 +3592,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5">
       <c r="A119">
         <v>168</v>
       </c>
@@ -3631,7 +3609,7 @@
         <v>1941</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5">
       <c r="A120">
         <v>213</v>
       </c>
@@ -3648,7 +3626,7 @@
         <v>1921</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5">
       <c r="A121">
         <v>24</v>
       </c>
@@ -3665,7 +3643,7 @@
         <v>1884</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5">
       <c r="A122">
         <v>47</v>
       </c>
@@ -3682,7 +3660,7 @@
         <v>1862</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5">
       <c r="A123">
         <v>19</v>
       </c>
@@ -3699,7 +3677,7 @@
         <v>1857</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5">
       <c r="A124">
         <v>33</v>
       </c>
@@ -3716,7 +3694,7 @@
         <v>1849</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5">
       <c r="A125">
         <v>178</v>
       </c>
@@ -3733,7 +3711,7 @@
         <v>1838</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5">
       <c r="A126">
         <v>221</v>
       </c>
@@ -3750,7 +3728,7 @@
         <v>1830</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5">
       <c r="A127">
         <v>59</v>
       </c>
@@ -3767,7 +3745,7 @@
         <v>1830</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5">
       <c r="A128">
         <v>235</v>
       </c>
@@ -3784,7 +3762,7 @@
         <v>1780</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5">
       <c r="A129">
         <v>170</v>
       </c>
@@ -3801,7 +3779,7 @@
         <v>1748</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5">
       <c r="A130">
         <v>111</v>
       </c>
@@ -3818,7 +3796,7 @@
         <v>1672</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5">
       <c r="A131">
         <v>147</v>
       </c>
@@ -3835,7 +3813,7 @@
         <v>1657</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5">
       <c r="A132">
         <v>169</v>
       </c>
@@ -3852,7 +3830,7 @@
         <v>1644</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5">
       <c r="A133">
         <v>26</v>
       </c>
@@ -3869,7 +3847,7 @@
         <v>1638</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5">
       <c r="A134">
         <v>131</v>
       </c>
@@ -3886,7 +3864,7 @@
         <v>1637</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5">
       <c r="A135">
         <v>218</v>
       </c>
@@ -3903,7 +3881,7 @@
         <v>1608</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5">
       <c r="A136">
         <v>110</v>
       </c>
@@ -3920,7 +3898,7 @@
         <v>1587</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:5">
       <c r="A137">
         <v>161</v>
       </c>
@@ -3937,7 +3915,7 @@
         <v>1581</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5">
       <c r="A138">
         <v>76</v>
       </c>
@@ -3954,7 +3932,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:5">
       <c r="A139">
         <v>194</v>
       </c>
@@ -3971,7 +3949,7 @@
         <v>1572</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5">
       <c r="A140">
         <v>66</v>
       </c>
@@ -3988,7 +3966,7 @@
         <v>1536</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:5">
       <c r="A141">
         <v>158</v>
       </c>
@@ -4005,7 +3983,7 @@
         <v>1509</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:5">
       <c r="A142">
         <v>188</v>
       </c>
@@ -4022,7 +4000,7 @@
         <v>1492</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5">
       <c r="A143">
         <v>27</v>
       </c>
@@ -4039,7 +4017,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:5">
       <c r="A144">
         <v>187</v>
       </c>
@@ -4056,7 +4034,7 @@
         <v>1484</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5">
       <c r="A145">
         <v>183</v>
       </c>
@@ -4073,7 +4051,7 @@
         <v>1478</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5">
       <c r="A146">
         <v>219</v>
       </c>
@@ -4090,7 +4068,7 @@
         <v>1476</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5">
       <c r="A147">
         <v>50</v>
       </c>
@@ -4107,7 +4085,7 @@
         <v>1471</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5">
       <c r="A148">
         <v>102</v>
       </c>
@@ -4124,7 +4102,7 @@
         <v>1457</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5">
       <c r="A149">
         <v>116</v>
       </c>
@@ -4141,7 +4119,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5">
       <c r="A150">
         <v>136</v>
       </c>
@@ -4158,7 +4136,7 @@
         <v>1424</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5">
       <c r="A151">
         <v>67</v>
       </c>
@@ -4175,7 +4153,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5">
       <c r="A152">
         <v>137</v>
       </c>
@@ -4192,7 +4170,7 @@
         <v>1396</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5">
       <c r="A153">
         <v>9</v>
       </c>
@@ -4209,7 +4187,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:5">
       <c r="A154">
         <v>149</v>
       </c>
@@ -4226,7 +4204,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5">
       <c r="A155">
         <v>78</v>
       </c>
@@ -4243,7 +4221,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:5">
       <c r="A156">
         <v>68</v>
       </c>
@@ -4260,7 +4238,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5">
       <c r="A157">
         <v>53</v>
       </c>
@@ -4277,7 +4255,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5">
       <c r="A158">
         <v>101</v>
       </c>
@@ -4294,7 +4272,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5">
       <c r="A159">
         <v>242</v>
       </c>
@@ -4311,7 +4289,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:5">
       <c r="A160">
         <v>117</v>
       </c>
@@ -4328,7 +4306,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:5">
       <c r="A161">
         <v>240</v>
       </c>
@@ -4345,7 +4323,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:5">
       <c r="A162">
         <v>28</v>
       </c>
@@ -4362,7 +4340,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:5">
       <c r="A163">
         <v>106</v>
       </c>
@@ -4379,7 +4357,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:5">
       <c r="A164">
         <v>86</v>
       </c>
@@ -4396,7 +4374,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:5">
       <c r="A165">
         <v>184</v>
       </c>
@@ -4413,7 +4391,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:5">
       <c r="A166">
         <v>208</v>
       </c>
@@ -4430,7 +4408,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5">
       <c r="A167">
         <v>60</v>
       </c>
@@ -4447,7 +4425,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:5">
       <c r="A168">
         <v>225</v>
       </c>
@@ -4464,7 +4442,7 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5">
       <c r="A169">
         <v>145</v>
       </c>
@@ -4481,7 +4459,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:5">
       <c r="A170">
         <v>1</v>
       </c>
@@ -4498,7 +4476,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:5">
       <c r="A171">
         <v>37</v>
       </c>
@@ -4515,7 +4493,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:5">
       <c r="A172">
         <v>91</v>
       </c>
@@ -4532,7 +4510,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:5">
       <c r="A173">
         <v>206</v>
       </c>
@@ -4549,7 +4527,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:5">
       <c r="A174">
         <v>79</v>
       </c>
@@ -4566,7 +4544,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:5">
       <c r="A175">
         <v>180</v>
       </c>
@@ -4583,7 +4561,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:5">
       <c r="A176">
         <v>171</v>
       </c>
@@ -4600,7 +4578,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:5">
       <c r="A177">
         <v>226</v>
       </c>
@@ -4617,7 +4595,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5">
       <c r="A178">
         <v>190</v>
       </c>
@@ -4634,7 +4612,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5">
       <c r="A179">
         <v>127</v>
       </c>
@@ -4651,7 +4629,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5">
       <c r="A180">
         <v>82</v>
       </c>
@@ -4668,7 +4646,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:5">
       <c r="A181">
         <v>126</v>
       </c>
@@ -4685,7 +4663,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5">
       <c r="A182">
         <v>157</v>
       </c>
@@ -4702,7 +4680,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5">
       <c r="A183">
         <v>216</v>
       </c>
@@ -4719,7 +4697,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5">
       <c r="A184">
         <v>129</v>
       </c>
@@ -4736,7 +4714,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5">
       <c r="A185">
         <v>89</v>
       </c>
@@ -4753,7 +4731,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5">
       <c r="A186">
         <v>128</v>
       </c>
@@ -4770,7 +4748,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5">
       <c r="A187">
         <v>182</v>
       </c>
@@ -4787,7 +4765,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:5">
       <c r="A188">
         <v>3</v>
       </c>
@@ -4804,7 +4782,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:5">
       <c r="A189">
         <v>55</v>
       </c>
@@ -4821,7 +4799,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5">
       <c r="A190">
         <v>93</v>
       </c>
@@ -4838,7 +4816,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:5">
       <c r="A191">
         <v>42</v>
       </c>
@@ -4855,7 +4833,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5">
       <c r="A192">
         <v>233</v>
       </c>
@@ -4872,7 +4850,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:5">
       <c r="A193">
         <v>205</v>
       </c>
@@ -4889,7 +4867,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:5">
       <c r="A194">
         <v>34</v>
       </c>
@@ -4906,7 +4884,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:5">
       <c r="A195">
         <v>154</v>
       </c>
@@ -4923,7 +4901,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:5">
       <c r="A196">
         <v>36</v>
       </c>
@@ -4940,7 +4918,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:5">
       <c r="A197">
         <v>236</v>
       </c>
@@ -4957,7 +4935,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:5">
       <c r="A198">
         <v>49</v>
       </c>
@@ -4974,7 +4952,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:5">
       <c r="A199">
         <v>143</v>
       </c>
@@ -4991,7 +4969,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:5">
       <c r="A200">
         <v>41</v>
       </c>
@@ -5008,7 +4986,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:5">
       <c r="A201">
         <v>132</v>
       </c>
@@ -5025,7 +5003,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:5">
       <c r="A202">
         <v>211</v>
       </c>
@@ -5042,7 +5020,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:5">
       <c r="A203">
         <v>94</v>
       </c>
@@ -5059,7 +5037,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:5">
       <c r="A204">
         <v>23</v>
       </c>
@@ -5076,7 +5054,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:5">
       <c r="A205">
         <v>121</v>
       </c>
@@ -5093,7 +5071,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:5">
       <c r="A206">
         <v>120</v>
       </c>
@@ -5110,7 +5088,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:5">
       <c r="A207">
         <v>96</v>
       </c>
@@ -5127,7 +5105,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:5">
       <c r="A208">
         <v>7</v>
       </c>
@@ -5144,7 +5122,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:5">
       <c r="A209">
         <v>232</v>
       </c>
@@ -5161,7 +5139,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:5">
       <c r="A210">
         <v>64</v>
       </c>
@@ -5178,7 +5156,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:5">
       <c r="A211">
         <v>18</v>
       </c>
@@ -5195,7 +5173,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:5">
       <c r="A212">
         <v>31</v>
       </c>
@@ -5212,7 +5190,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:5">
       <c r="A213">
         <v>156</v>
       </c>
@@ -5229,7 +5207,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:5">
       <c r="A214">
         <v>241</v>
       </c>
@@ -5246,7 +5224,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:5">
       <c r="A215">
         <v>35</v>
       </c>
@@ -5263,7 +5241,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:5">
       <c r="A216">
         <v>204</v>
       </c>
@@ -5280,7 +5258,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:5">
       <c r="A217">
         <v>239</v>
       </c>
@@ -5297,7 +5275,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:5">
       <c r="A218">
         <v>8</v>
       </c>
@@ -5314,7 +5292,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:5">
       <c r="A219">
         <v>164</v>
       </c>
@@ -5331,7 +5309,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:5">
       <c r="A220">
         <v>195</v>
       </c>
@@ -5348,7 +5326,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:5">
       <c r="A221">
         <v>231</v>
       </c>
@@ -5365,7 +5343,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:5">
       <c r="A222">
         <v>92</v>
       </c>
@@ -5382,7 +5360,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:5">
       <c r="A223">
         <v>214</v>
       </c>
@@ -5399,7 +5377,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:5">
       <c r="A224">
         <v>25</v>
       </c>
@@ -5416,7 +5394,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:5">
       <c r="A225">
         <v>200</v>
       </c>
@@ -5433,7 +5411,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:5">
       <c r="A226">
         <v>223</v>
       </c>
@@ -5450,7 +5428,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:5">
       <c r="A227">
         <v>61</v>
       </c>
@@ -5467,7 +5445,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:5">
       <c r="A228">
         <v>151</v>
       </c>
@@ -5484,7 +5462,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:5">
       <c r="A229">
         <v>148</v>
       </c>
@@ -5501,7 +5479,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:5">
       <c r="A230">
         <v>113</v>
       </c>
@@ -5518,7 +5496,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:5">
       <c r="A231">
         <v>10</v>
       </c>
@@ -5535,7 +5513,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:5">
       <c r="A232">
         <v>69</v>
       </c>
@@ -5552,7 +5530,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:5">
       <c r="A233">
         <v>100</v>
       </c>
@@ -5569,7 +5547,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:5">
       <c r="A234">
         <v>65</v>
       </c>
@@ -5586,7 +5564,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:5">
       <c r="A235">
         <v>140</v>
       </c>
@@ -5603,7 +5581,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:5">
       <c r="A236">
         <v>62</v>
       </c>
@@ -5620,7 +5598,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:5">
       <c r="A237">
         <v>63</v>
       </c>
@@ -5637,7 +5615,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:5">
       <c r="A238">
         <v>243</v>
       </c>
@@ -5654,7 +5632,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:5">
       <c r="A239">
         <v>5</v>
       </c>
@@ -5671,7 +5649,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:5">
       <c r="A240">
         <v>165</v>
       </c>
@@ -5688,7 +5666,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:5">
       <c r="A241">
         <v>166</v>
       </c>
@@ -5705,7 +5683,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:5">
       <c r="A242">
         <v>237</v>
       </c>
@@ -5722,7 +5700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:5">
       <c r="A243">
         <v>238</v>
       </c>

</xml_diff>